<commit_message>
EPBDS-6613 Add null-safety for 'power' operation
--HG--
branch : 5.19.x
</commit_message>
<xml_diff>
--- a/DEV/org.openl.test/test-resources/functionality/Arithmetic.xlsx
+++ b/DEV/org.openl.test/test-resources/functionality/Arithmetic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16935" windowHeight="7245" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16935" windowHeight="7245" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="12" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Sub" sheetId="15" r:id="rId3"/>
     <sheet name="Mul" sheetId="16" r:id="rId4"/>
     <sheet name="Div" sheetId="17" r:id="rId5"/>
+    <sheet name="Pow" sheetId="18" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="168">
   <si>
     <t>Result</t>
   </si>
@@ -514,6 +515,15 @@
   <si>
     <t>Test div div0Test</t>
   </si>
+  <si>
+    <t>= # ** #</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult pow (long v1, double v2, Long v3, Double v4, BigInteger v5, BigDecimal v6)</t>
+  </si>
+  <si>
+    <t>Test pow pow0Test</t>
+  </si>
 </sst>
 </file>
 
@@ -697,10 +707,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -992,7 +1002,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2232,32 +2242,32 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="H4" s="6"/>
@@ -5577,7 +5587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AE38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5610,32 +5620,32 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="H4" s="6"/>
@@ -7028,7 +7038,7 @@
         <v>= $X$BI1 - $FV2$Y</v>
       </c>
       <c r="AC18" s="7" t="str">
-        <f t="shared" ref="AC18:AW27" si="2">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H18,1),"#","$"&amp;AC$4&amp;"$Y",1)</f>
+        <f t="shared" ref="AC18:AE18" si="2">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H18,1),"#","$"&amp;AC$4&amp;"$Y",1)</f>
         <v>= $X$BI1 - $DV2$Y</v>
       </c>
       <c r="AD18" s="7" t="str">
@@ -7112,7 +7122,7 @@
         <v>= $X$BD1 - $SV2$Y</v>
       </c>
       <c r="Z19" s="7" t="str">
-        <f t="shared" ref="Z19:AT28" si="3">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H19,1),"#","$"&amp;Z$4&amp;"$Y",1)</f>
+        <f t="shared" ref="Z19:AE27" si="3">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H19,1),"#","$"&amp;Z$4&amp;"$Y",1)</f>
         <v>= $X$BD1 - $IV2$Y</v>
       </c>
       <c r="AA19" s="7" t="str">
@@ -8375,8 +8385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AE38"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8410,32 +8420,32 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="H4" s="6"/>
@@ -9828,7 +9838,7 @@
         <v>= $X$BI1 * $FV2$Y</v>
       </c>
       <c r="AC18" s="7" t="str">
-        <f t="shared" ref="AC18:AW27" si="2">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H18,1),"#","$"&amp;AC$4&amp;"$Y",1)</f>
+        <f t="shared" ref="AC18:AE18" si="2">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H18,1),"#","$"&amp;AC$4&amp;"$Y",1)</f>
         <v>= $X$BI1 * $DV2$Y</v>
       </c>
       <c r="AD18" s="7" t="str">
@@ -9912,7 +9922,7 @@
         <v>= $X$BD1 * $SV2$Y</v>
       </c>
       <c r="Z19" s="7" t="str">
-        <f t="shared" ref="Z19:AT28" si="3">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H19,1),"#","$"&amp;Z$4&amp;"$Y",1)</f>
+        <f t="shared" ref="Z19:AE27" si="3">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H19,1),"#","$"&amp;Z$4&amp;"$Y",1)</f>
         <v>= $X$BD1 * $IV2$Y</v>
       </c>
       <c r="AA19" s="7" t="str">
@@ -11175,7 +11185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AE38"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
@@ -11210,32 +11220,32 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="H4" s="6"/>
@@ -12628,7 +12638,7 @@
         <v>= $X$BI1 / $FV2$Y</v>
       </c>
       <c r="AC18" s="7" t="str">
-        <f t="shared" ref="AC18:AW27" si="2">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H18,1),"#","$"&amp;AC$4&amp;"$Y",1)</f>
+        <f t="shared" ref="AC18:AE18" si="2">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H18,1),"#","$"&amp;AC$4&amp;"$Y",1)</f>
         <v>= $X$BI1 / $DV2$Y</v>
       </c>
       <c r="AD18" s="7" t="str">
@@ -12712,7 +12722,7 @@
         <v>= $X$BD1 / $SV2$Y</v>
       </c>
       <c r="Z19" s="7" t="str">
-        <f t="shared" ref="Z19:AT28" si="3">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H19,1),"#","$"&amp;Z$4&amp;"$Y",1)</f>
+        <f t="shared" ref="Z19:AE27" si="3">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H19,1),"#","$"&amp;Z$4&amp;"$Y",1)</f>
         <v>= $X$BD1 / $IV2$Y</v>
       </c>
       <c r="AA19" s="7" t="str">
@@ -13957,6 +13967,2806 @@
       </c>
       <c r="AC38" s="1">
         <v>-3.3</v>
+      </c>
+      <c r="AE38" s="1">
+        <v>2.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="C32:H32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:AE38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC5" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE5" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="H6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="7" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H6,1),"#","$"&amp;J$4&amp;"$Y",1)</f>
+        <v>= $X$b1 ** $b2$Y</v>
+      </c>
+      <c r="K6" s="7" t="str">
+        <f t="shared" ref="K6:AE18" si="0">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H6,1),"#","$"&amp;K$4&amp;"$Y",1)</f>
+        <v>= $X$b1 ** $s2$Y</v>
+      </c>
+      <c r="L6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $i2$Y</v>
+      </c>
+      <c r="M6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $l2$Y</v>
+      </c>
+      <c r="N6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $f2$Y</v>
+      </c>
+      <c r="O6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $d2$Y</v>
+      </c>
+      <c r="P6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $B2$Y</v>
+      </c>
+      <c r="Q6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $S2$Y</v>
+      </c>
+      <c r="R6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $I2$Y</v>
+      </c>
+      <c r="S6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $L2$Y</v>
+      </c>
+      <c r="T6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $F2$Y</v>
+      </c>
+      <c r="U6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $D2$Y</v>
+      </c>
+      <c r="V6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $BI2$Y</v>
+      </c>
+      <c r="W6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $BD2$Y</v>
+      </c>
+      <c r="X6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $BV2$Y</v>
+      </c>
+      <c r="Y6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $SV2$Y</v>
+      </c>
+      <c r="Z6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $IV2$Y</v>
+      </c>
+      <c r="AA6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $LV2$Y</v>
+      </c>
+      <c r="AB6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $FV2$Y</v>
+      </c>
+      <c r="AC6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $DV2$Y</v>
+      </c>
+      <c r="AD6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$b1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="7" t="str">
+        <f t="shared" ref="J7:Y27" si="1">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H7,1),"#","$"&amp;J$4&amp;"$Y",1)</f>
+        <v>= $X$s1 ** $b2$Y</v>
+      </c>
+      <c r="K7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $s2$Y</v>
+      </c>
+      <c r="L7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $i2$Y</v>
+      </c>
+      <c r="M7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $l2$Y</v>
+      </c>
+      <c r="N7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $f2$Y</v>
+      </c>
+      <c r="O7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $d2$Y</v>
+      </c>
+      <c r="P7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $B2$Y</v>
+      </c>
+      <c r="Q7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $S2$Y</v>
+      </c>
+      <c r="R7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $I2$Y</v>
+      </c>
+      <c r="S7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $L2$Y</v>
+      </c>
+      <c r="T7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $F2$Y</v>
+      </c>
+      <c r="U7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $D2$Y</v>
+      </c>
+      <c r="V7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $BI2$Y</v>
+      </c>
+      <c r="W7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $BD2$Y</v>
+      </c>
+      <c r="X7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $BV2$Y</v>
+      </c>
+      <c r="Y7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$s1 ** $SV2$Y</v>
+      </c>
+      <c r="Z7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$s1 ** $IV2$Y</v>
+      </c>
+      <c r="AA7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$s1 ** $LV2$Y</v>
+      </c>
+      <c r="AB7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$s1 ** $FV2$Y</v>
+      </c>
+      <c r="AC7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$s1 ** $DV2$Y</v>
+      </c>
+      <c r="AD7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$s1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$s1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$i1 ** $b2$Y</v>
+      </c>
+      <c r="K8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $s2$Y</v>
+      </c>
+      <c r="L8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $i2$Y</v>
+      </c>
+      <c r="M8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $l2$Y</v>
+      </c>
+      <c r="N8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $f2$Y</v>
+      </c>
+      <c r="O8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $d2$Y</v>
+      </c>
+      <c r="P8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $B2$Y</v>
+      </c>
+      <c r="Q8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $S2$Y</v>
+      </c>
+      <c r="R8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $I2$Y</v>
+      </c>
+      <c r="S8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $L2$Y</v>
+      </c>
+      <c r="T8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $F2$Y</v>
+      </c>
+      <c r="U8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $D2$Y</v>
+      </c>
+      <c r="V8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $BI2$Y</v>
+      </c>
+      <c r="W8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $BD2$Y</v>
+      </c>
+      <c r="X8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $BV2$Y</v>
+      </c>
+      <c r="Y8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $SV2$Y</v>
+      </c>
+      <c r="Z8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $IV2$Y</v>
+      </c>
+      <c r="AA8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $LV2$Y</v>
+      </c>
+      <c r="AB8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $FV2$Y</v>
+      </c>
+      <c r="AC8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $DV2$Y</v>
+      </c>
+      <c r="AD8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$i1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$l1 ** $b2$Y</v>
+      </c>
+      <c r="K9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $s2$Y</v>
+      </c>
+      <c r="L9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $i2$Y</v>
+      </c>
+      <c r="M9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $l2$Y</v>
+      </c>
+      <c r="N9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $f2$Y</v>
+      </c>
+      <c r="O9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $d2$Y</v>
+      </c>
+      <c r="P9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $B2$Y</v>
+      </c>
+      <c r="Q9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $S2$Y</v>
+      </c>
+      <c r="R9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $I2$Y</v>
+      </c>
+      <c r="S9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $L2$Y</v>
+      </c>
+      <c r="T9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $F2$Y</v>
+      </c>
+      <c r="U9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $D2$Y</v>
+      </c>
+      <c r="V9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $BI2$Y</v>
+      </c>
+      <c r="W9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $BD2$Y</v>
+      </c>
+      <c r="X9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $BV2$Y</v>
+      </c>
+      <c r="Y9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $SV2$Y</v>
+      </c>
+      <c r="Z9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $IV2$Y</v>
+      </c>
+      <c r="AA9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $LV2$Y</v>
+      </c>
+      <c r="AB9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $FV2$Y</v>
+      </c>
+      <c r="AC9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $DV2$Y</v>
+      </c>
+      <c r="AD9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$l1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$f1 ** $b2$Y</v>
+      </c>
+      <c r="K10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $s2$Y</v>
+      </c>
+      <c r="L10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $i2$Y</v>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $l2$Y</v>
+      </c>
+      <c r="N10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $f2$Y</v>
+      </c>
+      <c r="O10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $d2$Y</v>
+      </c>
+      <c r="P10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $B2$Y</v>
+      </c>
+      <c r="Q10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $S2$Y</v>
+      </c>
+      <c r="R10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $I2$Y</v>
+      </c>
+      <c r="S10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $L2$Y</v>
+      </c>
+      <c r="T10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $F2$Y</v>
+      </c>
+      <c r="U10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $D2$Y</v>
+      </c>
+      <c r="V10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $BI2$Y</v>
+      </c>
+      <c r="W10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $BD2$Y</v>
+      </c>
+      <c r="X10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $BV2$Y</v>
+      </c>
+      <c r="Y10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $SV2$Y</v>
+      </c>
+      <c r="Z10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $IV2$Y</v>
+      </c>
+      <c r="AA10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $LV2$Y</v>
+      </c>
+      <c r="AB10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $FV2$Y</v>
+      </c>
+      <c r="AC10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $DV2$Y</v>
+      </c>
+      <c r="AD10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$f1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$d1 ** $b2$Y</v>
+      </c>
+      <c r="K11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $s2$Y</v>
+      </c>
+      <c r="L11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $i2$Y</v>
+      </c>
+      <c r="M11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $l2$Y</v>
+      </c>
+      <c r="N11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $f2$Y</v>
+      </c>
+      <c r="O11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $d2$Y</v>
+      </c>
+      <c r="P11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $B2$Y</v>
+      </c>
+      <c r="Q11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $S2$Y</v>
+      </c>
+      <c r="R11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $I2$Y</v>
+      </c>
+      <c r="S11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $L2$Y</v>
+      </c>
+      <c r="T11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $F2$Y</v>
+      </c>
+      <c r="U11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $D2$Y</v>
+      </c>
+      <c r="V11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $BI2$Y</v>
+      </c>
+      <c r="W11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $BD2$Y</v>
+      </c>
+      <c r="X11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $BV2$Y</v>
+      </c>
+      <c r="Y11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $SV2$Y</v>
+      </c>
+      <c r="Z11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $IV2$Y</v>
+      </c>
+      <c r="AA11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $LV2$Y</v>
+      </c>
+      <c r="AB11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $FV2$Y</v>
+      </c>
+      <c r="AC11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $DV2$Y</v>
+      </c>
+      <c r="AD11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$d1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="H12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$B1 ** $b2$Y</v>
+      </c>
+      <c r="K12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $s2$Y</v>
+      </c>
+      <c r="L12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $i2$Y</v>
+      </c>
+      <c r="M12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $l2$Y</v>
+      </c>
+      <c r="N12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $f2$Y</v>
+      </c>
+      <c r="O12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $d2$Y</v>
+      </c>
+      <c r="P12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $B2$Y</v>
+      </c>
+      <c r="Q12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $S2$Y</v>
+      </c>
+      <c r="R12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $I2$Y</v>
+      </c>
+      <c r="S12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $L2$Y</v>
+      </c>
+      <c r="T12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $F2$Y</v>
+      </c>
+      <c r="U12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $D2$Y</v>
+      </c>
+      <c r="V12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $BI2$Y</v>
+      </c>
+      <c r="W12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $BD2$Y</v>
+      </c>
+      <c r="X12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $BV2$Y</v>
+      </c>
+      <c r="Y12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $SV2$Y</v>
+      </c>
+      <c r="Z12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $IV2$Y</v>
+      </c>
+      <c r="AA12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $LV2$Y</v>
+      </c>
+      <c r="AB12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $FV2$Y</v>
+      </c>
+      <c r="AC12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $DV2$Y</v>
+      </c>
+      <c r="AD12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$B1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$S1 ** $b2$Y</v>
+      </c>
+      <c r="K13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $s2$Y</v>
+      </c>
+      <c r="L13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $i2$Y</v>
+      </c>
+      <c r="M13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $l2$Y</v>
+      </c>
+      <c r="N13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $f2$Y</v>
+      </c>
+      <c r="O13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $d2$Y</v>
+      </c>
+      <c r="P13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $B2$Y</v>
+      </c>
+      <c r="Q13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $S2$Y</v>
+      </c>
+      <c r="R13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $I2$Y</v>
+      </c>
+      <c r="S13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $L2$Y</v>
+      </c>
+      <c r="T13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $F2$Y</v>
+      </c>
+      <c r="U13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $D2$Y</v>
+      </c>
+      <c r="V13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $BI2$Y</v>
+      </c>
+      <c r="W13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $BD2$Y</v>
+      </c>
+      <c r="X13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $BV2$Y</v>
+      </c>
+      <c r="Y13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $SV2$Y</v>
+      </c>
+      <c r="Z13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $IV2$Y</v>
+      </c>
+      <c r="AA13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $LV2$Y</v>
+      </c>
+      <c r="AB13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $FV2$Y</v>
+      </c>
+      <c r="AC13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $DV2$Y</v>
+      </c>
+      <c r="AD13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$S1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J14" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$I1 ** $b2$Y</v>
+      </c>
+      <c r="K14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $s2$Y</v>
+      </c>
+      <c r="L14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $i2$Y</v>
+      </c>
+      <c r="M14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $l2$Y</v>
+      </c>
+      <c r="N14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $f2$Y</v>
+      </c>
+      <c r="O14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $d2$Y</v>
+      </c>
+      <c r="P14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $B2$Y</v>
+      </c>
+      <c r="Q14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $S2$Y</v>
+      </c>
+      <c r="R14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $I2$Y</v>
+      </c>
+      <c r="S14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $L2$Y</v>
+      </c>
+      <c r="T14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $F2$Y</v>
+      </c>
+      <c r="U14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $D2$Y</v>
+      </c>
+      <c r="V14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $BI2$Y</v>
+      </c>
+      <c r="W14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $BD2$Y</v>
+      </c>
+      <c r="X14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $BV2$Y</v>
+      </c>
+      <c r="Y14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $SV2$Y</v>
+      </c>
+      <c r="Z14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $IV2$Y</v>
+      </c>
+      <c r="AA14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $LV2$Y</v>
+      </c>
+      <c r="AB14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $FV2$Y</v>
+      </c>
+      <c r="AC14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $DV2$Y</v>
+      </c>
+      <c r="AD14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$I1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$L1 ** $b2$Y</v>
+      </c>
+      <c r="K15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $s2$Y</v>
+      </c>
+      <c r="L15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $i2$Y</v>
+      </c>
+      <c r="M15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $l2$Y</v>
+      </c>
+      <c r="N15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $f2$Y</v>
+      </c>
+      <c r="O15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $d2$Y</v>
+      </c>
+      <c r="P15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $B2$Y</v>
+      </c>
+      <c r="Q15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $S2$Y</v>
+      </c>
+      <c r="R15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $I2$Y</v>
+      </c>
+      <c r="S15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $L2$Y</v>
+      </c>
+      <c r="T15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $F2$Y</v>
+      </c>
+      <c r="U15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $D2$Y</v>
+      </c>
+      <c r="V15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $BI2$Y</v>
+      </c>
+      <c r="W15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $BD2$Y</v>
+      </c>
+      <c r="X15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $BV2$Y</v>
+      </c>
+      <c r="Y15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $SV2$Y</v>
+      </c>
+      <c r="Z15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $IV2$Y</v>
+      </c>
+      <c r="AA15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $LV2$Y</v>
+      </c>
+      <c r="AB15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $FV2$Y</v>
+      </c>
+      <c r="AC15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $DV2$Y</v>
+      </c>
+      <c r="AD15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$L1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="H16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$F1 ** $b2$Y</v>
+      </c>
+      <c r="K16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $s2$Y</v>
+      </c>
+      <c r="L16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $i2$Y</v>
+      </c>
+      <c r="M16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $l2$Y</v>
+      </c>
+      <c r="N16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $f2$Y</v>
+      </c>
+      <c r="O16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $d2$Y</v>
+      </c>
+      <c r="P16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $B2$Y</v>
+      </c>
+      <c r="Q16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $S2$Y</v>
+      </c>
+      <c r="R16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $I2$Y</v>
+      </c>
+      <c r="S16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $L2$Y</v>
+      </c>
+      <c r="T16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $F2$Y</v>
+      </c>
+      <c r="U16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $D2$Y</v>
+      </c>
+      <c r="V16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $BI2$Y</v>
+      </c>
+      <c r="W16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $BD2$Y</v>
+      </c>
+      <c r="X16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $BV2$Y</v>
+      </c>
+      <c r="Y16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $SV2$Y</v>
+      </c>
+      <c r="Z16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $IV2$Y</v>
+      </c>
+      <c r="AA16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $LV2$Y</v>
+      </c>
+      <c r="AB16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $FV2$Y</v>
+      </c>
+      <c r="AC16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $DV2$Y</v>
+      </c>
+      <c r="AD16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$F1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="17" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="H17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$D1 ** $b2$Y</v>
+      </c>
+      <c r="K17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $s2$Y</v>
+      </c>
+      <c r="L17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $i2$Y</v>
+      </c>
+      <c r="M17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $l2$Y</v>
+      </c>
+      <c r="N17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $f2$Y</v>
+      </c>
+      <c r="O17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $d2$Y</v>
+      </c>
+      <c r="P17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $B2$Y</v>
+      </c>
+      <c r="Q17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $S2$Y</v>
+      </c>
+      <c r="R17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $I2$Y</v>
+      </c>
+      <c r="S17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $L2$Y</v>
+      </c>
+      <c r="T17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $F2$Y</v>
+      </c>
+      <c r="U17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $D2$Y</v>
+      </c>
+      <c r="V17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $BI2$Y</v>
+      </c>
+      <c r="W17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $BD2$Y</v>
+      </c>
+      <c r="X17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $BV2$Y</v>
+      </c>
+      <c r="Y17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $SV2$Y</v>
+      </c>
+      <c r="Z17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $IV2$Y</v>
+      </c>
+      <c r="AA17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $LV2$Y</v>
+      </c>
+      <c r="AB17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $FV2$Y</v>
+      </c>
+      <c r="AC17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $DV2$Y</v>
+      </c>
+      <c r="AD17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$D1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="18" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="H18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J18" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BI1 ** $b2$Y</v>
+      </c>
+      <c r="K18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $s2$Y</v>
+      </c>
+      <c r="L18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $i2$Y</v>
+      </c>
+      <c r="M18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $l2$Y</v>
+      </c>
+      <c r="N18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $f2$Y</v>
+      </c>
+      <c r="O18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $d2$Y</v>
+      </c>
+      <c r="P18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $B2$Y</v>
+      </c>
+      <c r="Q18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $S2$Y</v>
+      </c>
+      <c r="R18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $I2$Y</v>
+      </c>
+      <c r="S18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $L2$Y</v>
+      </c>
+      <c r="T18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $F2$Y</v>
+      </c>
+      <c r="U18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $D2$Y</v>
+      </c>
+      <c r="V18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $BI2$Y</v>
+      </c>
+      <c r="W18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $BD2$Y</v>
+      </c>
+      <c r="X18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $BV2$Y</v>
+      </c>
+      <c r="Y18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $SV2$Y</v>
+      </c>
+      <c r="Z18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $IV2$Y</v>
+      </c>
+      <c r="AA18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $LV2$Y</v>
+      </c>
+      <c r="AB18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>= $X$BI1 ** $FV2$Y</v>
+      </c>
+      <c r="AC18" s="7" t="str">
+        <f t="shared" ref="AC18:AE18" si="2">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H18,1),"#","$"&amp;AC$4&amp;"$Y",1)</f>
+        <v>= $X$BI1 ** $DV2$Y</v>
+      </c>
+      <c r="AD18" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>= $X$BI1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE18" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>= $X$BI1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="19" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="H19" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $b2$Y</v>
+      </c>
+      <c r="K19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $s2$Y</v>
+      </c>
+      <c r="L19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $i2$Y</v>
+      </c>
+      <c r="M19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $l2$Y</v>
+      </c>
+      <c r="N19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $f2$Y</v>
+      </c>
+      <c r="O19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $d2$Y</v>
+      </c>
+      <c r="P19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $B2$Y</v>
+      </c>
+      <c r="Q19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $S2$Y</v>
+      </c>
+      <c r="R19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $I2$Y</v>
+      </c>
+      <c r="S19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $L2$Y</v>
+      </c>
+      <c r="T19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $F2$Y</v>
+      </c>
+      <c r="U19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $D2$Y</v>
+      </c>
+      <c r="V19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $BI2$Y</v>
+      </c>
+      <c r="W19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $BD2$Y</v>
+      </c>
+      <c r="X19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $BV2$Y</v>
+      </c>
+      <c r="Y19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BD1 ** $SV2$Y</v>
+      </c>
+      <c r="Z19" s="7" t="str">
+        <f t="shared" ref="Z19:AE27" si="3">SUBSTITUTE(SUBSTITUTE($A$6,"#","$X$"&amp;$H19,1),"#","$"&amp;Z$4&amp;"$Y",1)</f>
+        <v>= $X$BD1 ** $IV2$Y</v>
+      </c>
+      <c r="AA19" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BD1 ** $LV2$Y</v>
+      </c>
+      <c r="AB19" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BD1 ** $FV2$Y</v>
+      </c>
+      <c r="AC19" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BD1 ** $DV2$Y</v>
+      </c>
+      <c r="AD19" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BD1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE19" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BD1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="20" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="H20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $b2$Y</v>
+      </c>
+      <c r="K20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $s2$Y</v>
+      </c>
+      <c r="L20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $i2$Y</v>
+      </c>
+      <c r="M20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $l2$Y</v>
+      </c>
+      <c r="N20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $f2$Y</v>
+      </c>
+      <c r="O20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $d2$Y</v>
+      </c>
+      <c r="P20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $B2$Y</v>
+      </c>
+      <c r="Q20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $S2$Y</v>
+      </c>
+      <c r="R20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $I2$Y</v>
+      </c>
+      <c r="S20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $L2$Y</v>
+      </c>
+      <c r="T20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $F2$Y</v>
+      </c>
+      <c r="U20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $D2$Y</v>
+      </c>
+      <c r="V20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $BI2$Y</v>
+      </c>
+      <c r="W20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $BD2$Y</v>
+      </c>
+      <c r="X20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $BV2$Y</v>
+      </c>
+      <c r="Y20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BV1 ** $SV2$Y</v>
+      </c>
+      <c r="Z20" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BV1 ** $IV2$Y</v>
+      </c>
+      <c r="AA20" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BV1 ** $LV2$Y</v>
+      </c>
+      <c r="AB20" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BV1 ** $FV2$Y</v>
+      </c>
+      <c r="AC20" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BV1 ** $DV2$Y</v>
+      </c>
+      <c r="AD20" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BV1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE20" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BV1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="21" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="H21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $b2$Y</v>
+      </c>
+      <c r="K21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $s2$Y</v>
+      </c>
+      <c r="L21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $i2$Y</v>
+      </c>
+      <c r="M21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $l2$Y</v>
+      </c>
+      <c r="N21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $f2$Y</v>
+      </c>
+      <c r="O21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $d2$Y</v>
+      </c>
+      <c r="P21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $B2$Y</v>
+      </c>
+      <c r="Q21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $S2$Y</v>
+      </c>
+      <c r="R21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $I2$Y</v>
+      </c>
+      <c r="S21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $L2$Y</v>
+      </c>
+      <c r="T21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $F2$Y</v>
+      </c>
+      <c r="U21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $D2$Y</v>
+      </c>
+      <c r="V21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $BI2$Y</v>
+      </c>
+      <c r="W21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $BD2$Y</v>
+      </c>
+      <c r="X21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $BV2$Y</v>
+      </c>
+      <c r="Y21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$SV1 ** $SV2$Y</v>
+      </c>
+      <c r="Z21" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$SV1 ** $IV2$Y</v>
+      </c>
+      <c r="AA21" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$SV1 ** $LV2$Y</v>
+      </c>
+      <c r="AB21" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$SV1 ** $FV2$Y</v>
+      </c>
+      <c r="AC21" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$SV1 ** $DV2$Y</v>
+      </c>
+      <c r="AD21" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$SV1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE21" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$SV1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="22" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="H22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $b2$Y</v>
+      </c>
+      <c r="K22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $s2$Y</v>
+      </c>
+      <c r="L22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $i2$Y</v>
+      </c>
+      <c r="M22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $l2$Y</v>
+      </c>
+      <c r="N22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $f2$Y</v>
+      </c>
+      <c r="O22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $d2$Y</v>
+      </c>
+      <c r="P22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $B2$Y</v>
+      </c>
+      <c r="Q22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $S2$Y</v>
+      </c>
+      <c r="R22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $I2$Y</v>
+      </c>
+      <c r="S22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $L2$Y</v>
+      </c>
+      <c r="T22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $F2$Y</v>
+      </c>
+      <c r="U22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $D2$Y</v>
+      </c>
+      <c r="V22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $BI2$Y</v>
+      </c>
+      <c r="W22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $BD2$Y</v>
+      </c>
+      <c r="X22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $BV2$Y</v>
+      </c>
+      <c r="Y22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$IV1 ** $SV2$Y</v>
+      </c>
+      <c r="Z22" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$IV1 ** $IV2$Y</v>
+      </c>
+      <c r="AA22" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$IV1 ** $LV2$Y</v>
+      </c>
+      <c r="AB22" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$IV1 ** $FV2$Y</v>
+      </c>
+      <c r="AC22" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$IV1 ** $DV2$Y</v>
+      </c>
+      <c r="AD22" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$IV1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE22" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$IV1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="23" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="H23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $b2$Y</v>
+      </c>
+      <c r="K23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $s2$Y</v>
+      </c>
+      <c r="L23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $i2$Y</v>
+      </c>
+      <c r="M23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $l2$Y</v>
+      </c>
+      <c r="N23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $f2$Y</v>
+      </c>
+      <c r="O23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $d2$Y</v>
+      </c>
+      <c r="P23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $B2$Y</v>
+      </c>
+      <c r="Q23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $S2$Y</v>
+      </c>
+      <c r="R23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $I2$Y</v>
+      </c>
+      <c r="S23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $L2$Y</v>
+      </c>
+      <c r="T23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $F2$Y</v>
+      </c>
+      <c r="U23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $D2$Y</v>
+      </c>
+      <c r="V23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $BI2$Y</v>
+      </c>
+      <c r="W23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $BD2$Y</v>
+      </c>
+      <c r="X23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $BV2$Y</v>
+      </c>
+      <c r="Y23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$LV1 ** $SV2$Y</v>
+      </c>
+      <c r="Z23" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$LV1 ** $IV2$Y</v>
+      </c>
+      <c r="AA23" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$LV1 ** $LV2$Y</v>
+      </c>
+      <c r="AB23" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$LV1 ** $FV2$Y</v>
+      </c>
+      <c r="AC23" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$LV1 ** $DV2$Y</v>
+      </c>
+      <c r="AD23" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$LV1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE23" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$LV1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="24" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="H24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $b2$Y</v>
+      </c>
+      <c r="K24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $s2$Y</v>
+      </c>
+      <c r="L24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $i2$Y</v>
+      </c>
+      <c r="M24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $l2$Y</v>
+      </c>
+      <c r="N24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $f2$Y</v>
+      </c>
+      <c r="O24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $d2$Y</v>
+      </c>
+      <c r="P24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $B2$Y</v>
+      </c>
+      <c r="Q24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $S2$Y</v>
+      </c>
+      <c r="R24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $I2$Y</v>
+      </c>
+      <c r="S24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $L2$Y</v>
+      </c>
+      <c r="T24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $F2$Y</v>
+      </c>
+      <c r="U24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $D2$Y</v>
+      </c>
+      <c r="V24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $BI2$Y</v>
+      </c>
+      <c r="W24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $BD2$Y</v>
+      </c>
+      <c r="X24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $BV2$Y</v>
+      </c>
+      <c r="Y24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$FV1 ** $SV2$Y</v>
+      </c>
+      <c r="Z24" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$FV1 ** $IV2$Y</v>
+      </c>
+      <c r="AA24" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$FV1 ** $LV2$Y</v>
+      </c>
+      <c r="AB24" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$FV1 ** $FV2$Y</v>
+      </c>
+      <c r="AC24" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$FV1 ** $DV2$Y</v>
+      </c>
+      <c r="AD24" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$FV1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE24" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$FV1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="25" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="H25" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $b2$Y</v>
+      </c>
+      <c r="K25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $s2$Y</v>
+      </c>
+      <c r="L25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $i2$Y</v>
+      </c>
+      <c r="M25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $l2$Y</v>
+      </c>
+      <c r="N25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $f2$Y</v>
+      </c>
+      <c r="O25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $d2$Y</v>
+      </c>
+      <c r="P25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $B2$Y</v>
+      </c>
+      <c r="Q25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $S2$Y</v>
+      </c>
+      <c r="R25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $I2$Y</v>
+      </c>
+      <c r="S25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $L2$Y</v>
+      </c>
+      <c r="T25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $F2$Y</v>
+      </c>
+      <c r="U25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $D2$Y</v>
+      </c>
+      <c r="V25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $BI2$Y</v>
+      </c>
+      <c r="W25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $BD2$Y</v>
+      </c>
+      <c r="X25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $BV2$Y</v>
+      </c>
+      <c r="Y25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$DV1 ** $SV2$Y</v>
+      </c>
+      <c r="Z25" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$DV1 ** $IV2$Y</v>
+      </c>
+      <c r="AA25" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$DV1 ** $LV2$Y</v>
+      </c>
+      <c r="AB25" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$DV1 ** $FV2$Y</v>
+      </c>
+      <c r="AC25" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$DV1 ** $DV2$Y</v>
+      </c>
+      <c r="AD25" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$DV1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE25" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$DV1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="26" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="H26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $b2$Y</v>
+      </c>
+      <c r="K26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $s2$Y</v>
+      </c>
+      <c r="L26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $i2$Y</v>
+      </c>
+      <c r="M26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $l2$Y</v>
+      </c>
+      <c r="N26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $f2$Y</v>
+      </c>
+      <c r="O26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $d2$Y</v>
+      </c>
+      <c r="P26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $B2$Y</v>
+      </c>
+      <c r="Q26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $S2$Y</v>
+      </c>
+      <c r="R26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $I2$Y</v>
+      </c>
+      <c r="S26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $L2$Y</v>
+      </c>
+      <c r="T26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $F2$Y</v>
+      </c>
+      <c r="U26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $D2$Y</v>
+      </c>
+      <c r="V26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $BI2$Y</v>
+      </c>
+      <c r="W26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $BD2$Y</v>
+      </c>
+      <c r="X26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $BV2$Y</v>
+      </c>
+      <c r="Y26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BIV1 ** $SV2$Y</v>
+      </c>
+      <c r="Z26" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BIV1 ** $IV2$Y</v>
+      </c>
+      <c r="AA26" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BIV1 ** $LV2$Y</v>
+      </c>
+      <c r="AB26" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BIV1 ** $FV2$Y</v>
+      </c>
+      <c r="AC26" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BIV1 ** $DV2$Y</v>
+      </c>
+      <c r="AD26" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BIV1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE26" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BIV1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="27" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="H27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $b2$Y</v>
+      </c>
+      <c r="K27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $s2$Y</v>
+      </c>
+      <c r="L27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $i2$Y</v>
+      </c>
+      <c r="M27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $l2$Y</v>
+      </c>
+      <c r="N27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $f2$Y</v>
+      </c>
+      <c r="O27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $d2$Y</v>
+      </c>
+      <c r="P27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $B2$Y</v>
+      </c>
+      <c r="Q27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $S2$Y</v>
+      </c>
+      <c r="R27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $I2$Y</v>
+      </c>
+      <c r="S27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $L2$Y</v>
+      </c>
+      <c r="T27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $F2$Y</v>
+      </c>
+      <c r="U27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $D2$Y</v>
+      </c>
+      <c r="V27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $BI2$Y</v>
+      </c>
+      <c r="W27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $BD2$Y</v>
+      </c>
+      <c r="X27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $BV2$Y</v>
+      </c>
+      <c r="Y27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>= $X$BDV1 ** $SV2$Y</v>
+      </c>
+      <c r="Z27" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BDV1 ** $IV2$Y</v>
+      </c>
+      <c r="AA27" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BDV1 ** $LV2$Y</v>
+      </c>
+      <c r="AB27" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BDV1 ** $FV2$Y</v>
+      </c>
+      <c r="AC27" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BDV1 ** $DV2$Y</v>
+      </c>
+      <c r="AD27" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BDV1 ** $BIV2$Y</v>
+      </c>
+      <c r="AE27" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>= $X$BDV1 ** $BDV2$Y</v>
+      </c>
+    </row>
+    <row r="32" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C32" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I33" s="1" t="str">
+        <f>"_res_.$"&amp;I$4&amp;"$"&amp;$H5</f>
+        <v>_res_.$X$Y</v>
+      </c>
+      <c r="J33" s="1" t="str">
+        <f t="shared" ref="J33:AE33" si="4">"_res_.$"&amp;J$4&amp;"$"&amp;$H5</f>
+        <v>_res_.$b2$Y</v>
+      </c>
+      <c r="K33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$s2$Y</v>
+      </c>
+      <c r="L33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$i2$Y</v>
+      </c>
+      <c r="M33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$l2$Y</v>
+      </c>
+      <c r="N33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$f2$Y</v>
+      </c>
+      <c r="O33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$d2$Y</v>
+      </c>
+      <c r="P33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$B2$Y</v>
+      </c>
+      <c r="Q33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$S2$Y</v>
+      </c>
+      <c r="R33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$I2$Y</v>
+      </c>
+      <c r="S33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$L2$Y</v>
+      </c>
+      <c r="T33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$F2$Y</v>
+      </c>
+      <c r="U33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$D2$Y</v>
+      </c>
+      <c r="V33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$BI2$Y</v>
+      </c>
+      <c r="W33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$BD2$Y</v>
+      </c>
+      <c r="X33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$BV2$Y</v>
+      </c>
+      <c r="Y33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$SV2$Y</v>
+      </c>
+      <c r="Z33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$IV2$Y</v>
+      </c>
+      <c r="AA33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$LV2$Y</v>
+      </c>
+      <c r="AB33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$FV2$Y</v>
+      </c>
+      <c r="AC33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$DV2$Y</v>
+      </c>
+      <c r="AD33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$BIV2$Y</v>
+      </c>
+      <c r="AE33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>_res_.$BDV2$Y</v>
+      </c>
+    </row>
+    <row r="34" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f>I$4</f>
+        <v>X</v>
+      </c>
+      <c r="J34" s="1" t="str">
+        <f t="shared" ref="J34:AE34" si="5">J$4</f>
+        <v>b2</v>
+      </c>
+      <c r="K34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>s2</v>
+      </c>
+      <c r="L34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>i2</v>
+      </c>
+      <c r="M34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>l2</v>
+      </c>
+      <c r="N34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>f2</v>
+      </c>
+      <c r="O34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>d2</v>
+      </c>
+      <c r="P34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>B2</v>
+      </c>
+      <c r="Q34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>S2</v>
+      </c>
+      <c r="R34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>I2</v>
+      </c>
+      <c r="S34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>L2</v>
+      </c>
+      <c r="T34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>F2</v>
+      </c>
+      <c r="U34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>D2</v>
+      </c>
+      <c r="V34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>BI2</v>
+      </c>
+      <c r="W34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>BD2</v>
+      </c>
+      <c r="X34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>BV2</v>
+      </c>
+      <c r="Y34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>SV2</v>
+      </c>
+      <c r="Z34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>IV2</v>
+      </c>
+      <c r="AA34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>LV2</v>
+      </c>
+      <c r="AB34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>FV2</v>
+      </c>
+      <c r="AC34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>DV2</v>
+      </c>
+      <c r="AD34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>BIV2</v>
+      </c>
+      <c r="AE34" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>BDV2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C35" s="1">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E35" s="1">
+        <v>34</v>
+      </c>
+      <c r="F35" s="1">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="G35" s="1">
+        <v>67</v>
+      </c>
+      <c r="H35" s="1">
+        <v>13.65</v>
+      </c>
+      <c r="J35" s="1">
+        <v>3</v>
+      </c>
+      <c r="K35" s="1">
+        <v>3</v>
+      </c>
+      <c r="L35" s="1">
+        <v>3</v>
+      </c>
+      <c r="M35" s="1">
+        <v>3</v>
+      </c>
+      <c r="N35" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O35" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P35" s="1">
+        <v>34</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>34</v>
+      </c>
+      <c r="R35" s="1">
+        <v>34</v>
+      </c>
+      <c r="S35" s="1">
+        <v>34</v>
+      </c>
+      <c r="T35" s="1">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="U35" s="1">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="V35" s="1">
+        <v>67</v>
+      </c>
+      <c r="W35" s="1">
+        <v>13.65</v>
+      </c>
+      <c r="X35" s="1">
+        <v>34</v>
+      </c>
+      <c r="Y35" s="1">
+        <v>34</v>
+      </c>
+      <c r="Z35" s="1">
+        <v>34</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>34</v>
+      </c>
+      <c r="AB35" s="1">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="AD35" s="1">
+        <v>67</v>
+      </c>
+      <c r="AE35" s="1">
+        <v>13.65</v>
+      </c>
+    </row>
+    <row r="36" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C36" s="1">
+        <v>12</v>
+      </c>
+      <c r="D36" s="1">
+        <v>68.8</v>
+      </c>
+      <c r="J36" s="1">
+        <v>12</v>
+      </c>
+      <c r="K36" s="1">
+        <v>12</v>
+      </c>
+      <c r="L36" s="1">
+        <v>12</v>
+      </c>
+      <c r="M36" s="1">
+        <v>12</v>
+      </c>
+      <c r="N36" s="1">
+        <v>68.8</v>
+      </c>
+      <c r="O36" s="1">
+        <v>68.8</v>
+      </c>
+    </row>
+    <row r="37" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C37" s="1">
+        <v>15</v>
+      </c>
+      <c r="D37" s="1">
+        <v>17</v>
+      </c>
+      <c r="E37" s="1">
+        <v>5</v>
+      </c>
+      <c r="G37" s="1">
+        <v>7</v>
+      </c>
+      <c r="J37" s="1">
+        <v>15</v>
+      </c>
+      <c r="K37" s="1">
+        <v>15</v>
+      </c>
+      <c r="L37" s="1">
+        <v>15</v>
+      </c>
+      <c r="M37" s="1">
+        <v>15</v>
+      </c>
+      <c r="N37" s="1">
+        <v>17</v>
+      </c>
+      <c r="O37" s="1">
+        <v>17</v>
+      </c>
+      <c r="P37" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>5</v>
+      </c>
+      <c r="R37" s="1">
+        <v>5</v>
+      </c>
+      <c r="S37" s="1">
+        <v>5</v>
+      </c>
+      <c r="V37" s="1">
+        <v>7</v>
+      </c>
+      <c r="X37" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y37" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z37" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA37" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD37" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C38" s="1">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="F38" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="H38" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="J38" s="1">
+        <v>3</v>
+      </c>
+      <c r="K38" s="1">
+        <v>3</v>
+      </c>
+      <c r="L38" s="1">
+        <v>3</v>
+      </c>
+      <c r="M38" s="1">
+        <v>3</v>
+      </c>
+      <c r="N38" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="O38" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="T38" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="U38" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="W38" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AB38" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="AC38" s="1">
+        <v>3.3</v>
       </c>
       <c r="AE38" s="1">
         <v>2.6</v>

</xml_diff>